<commit_message>
Antes de montar en linux
</commit_message>
<xml_diff>
--- a/alerta.xlsx
+++ b/alerta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProyectoTesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C741A2F-5BF9-4BBC-B264-4E0E667FFF89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D80B08-D9F4-4E6D-8CF0-A427CDB415E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BD24CBCE-041D-42B7-B6C6-8D4A654C39E6}"/>
   </bookViews>
@@ -84,10 +84,17 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -113,13 +120,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,7 +445,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,22 +480,22 @@
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="4">
         <v>45282</v>
       </c>
     </row>

</xml_diff>